<commit_message>
Updated on 02-05-2024 at 22:47
</commit_message>
<xml_diff>
--- a/experiment_3/output/output_latex.xlsx
+++ b/experiment_3/output/output_latex.xlsx
@@ -491,7 +491,7 @@
         <v>0.127</v>
       </c>
       <c r="I2" t="n">
-        <v>0.577</v>
+        <v>0.527</v>
       </c>
       <c r="J2" t="n">
         <v>412</v>
@@ -526,7 +526,7 @@
         <v>0.079</v>
       </c>
       <c r="I3" t="n">
-        <v>0.549</v>
+        <v>0.516</v>
       </c>
       <c r="J3" t="n">
         <v>378</v>
@@ -561,7 +561,7 @@
         <v>0.105</v>
       </c>
       <c r="I4" t="n">
-        <v>0.676</v>
+        <v>0.597</v>
       </c>
       <c r="J4" t="n">
         <v>152</v>
@@ -596,7 +596,7 @@
         <v>0.152</v>
       </c>
       <c r="I5" t="n">
-        <v>0.699</v>
+        <v>0.614</v>
       </c>
       <c r="J5" t="n">
         <v>178</v>
@@ -631,7 +631,7 @@
         <v>0.127</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.601</v>
       </c>
       <c r="J6" t="n">
         <v>206</v>
@@ -666,7 +666,7 @@
         <v>0.082</v>
       </c>
       <c r="I7" t="n">
-        <v>0.645</v>
+        <v>0.576</v>
       </c>
       <c r="J7" t="n">
         <v>209</v>
@@ -701,7 +701,7 @@
         <v>0.054</v>
       </c>
       <c r="I8" t="n">
-        <v>0.648</v>
+        <v>0.582</v>
       </c>
       <c r="J8" t="n">
         <v>178</v>
@@ -736,7 +736,7 @@
         <v>0.024</v>
       </c>
       <c r="I9" t="n">
-        <v>0.636</v>
+        <v>0.574</v>
       </c>
       <c r="J9" t="n">
         <v>175</v>
@@ -771,7 +771,7 @@
         <v>0.024</v>
       </c>
       <c r="I10" t="n">
-        <v>0.639</v>
+        <v>0.575</v>
       </c>
       <c r="J10" t="n">
         <v>192</v>
@@ -806,7 +806,7 @@
         <v>0.025</v>
       </c>
       <c r="I11" t="n">
-        <v>0.629</v>
+        <v>0.569</v>
       </c>
       <c r="J11" t="n">
         <v>162</v>
@@ -841,7 +841,7 @@
         <v>0.029</v>
       </c>
       <c r="I12" t="n">
-        <v>0.615</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="J12" t="n">
         <v>142</v>

</xml_diff>

<commit_message>
Updated on 04-21-2024 at 13:27
</commit_message>
<xml_diff>
--- a/experiment_3/output/output_latex.xlsx
+++ b/experiment_3/output/output_latex.xlsx
@@ -491,13 +491,13 @@
         <v>0.127</v>
       </c>
       <c r="I2" t="n">
-        <v>0.527</v>
+        <v>0.295</v>
       </c>
       <c r="J2" t="n">
-        <v>412</v>
+        <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>1919</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -514,7 +514,7 @@
         <v>-3.003</v>
       </c>
       <c r="E3" t="n">
-        <v>1.005</v>
+        <v>1.006</v>
       </c>
       <c r="F3" t="n">
         <v>5.634</v>
@@ -526,13 +526,13 @@
         <v>0.079</v>
       </c>
       <c r="I3" t="n">
-        <v>0.516</v>
+        <v>0.356</v>
       </c>
       <c r="J3" t="n">
-        <v>378</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>1759</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -561,13 +561,13 @@
         <v>0.105</v>
       </c>
       <c r="I4" t="n">
-        <v>0.597</v>
+        <v>0.437</v>
       </c>
       <c r="J4" t="n">
-        <v>152</v>
+        <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>695</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -596,13 +596,13 @@
         <v>0.152</v>
       </c>
       <c r="I5" t="n">
-        <v>0.614</v>
+        <v>0.511</v>
       </c>
       <c r="J5" t="n">
-        <v>178</v>
+        <v>3</v>
       </c>
       <c r="K5" t="n">
-        <v>815</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -631,13 +631,13 @@
         <v>0.127</v>
       </c>
       <c r="I6" t="n">
-        <v>0.601</v>
+        <v>0.48</v>
       </c>
       <c r="J6" t="n">
-        <v>206</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>942</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -666,13 +666,13 @@
         <v>0.082</v>
       </c>
       <c r="I7" t="n">
-        <v>0.576</v>
+        <v>0.332</v>
       </c>
       <c r="J7" t="n">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="K7" t="n">
-        <v>957</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -701,13 +701,13 @@
         <v>0.054</v>
       </c>
       <c r="I8" t="n">
-        <v>0.582</v>
+        <v>0.283</v>
       </c>
       <c r="J8" t="n">
-        <v>178</v>
+        <v>3</v>
       </c>
       <c r="K8" t="n">
-        <v>812</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>0.981</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.976</v>
+        <v>-2.977</v>
       </c>
       <c r="E9" t="n">
         <v>0.993</v>
@@ -733,16 +733,16 @@
         <v>0.031</v>
       </c>
       <c r="H9" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="I9" t="n">
-        <v>0.574</v>
+        <v>0.28</v>
       </c>
       <c r="J9" t="n">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="K9" t="n">
-        <v>796</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -771,13 +771,13 @@
         <v>0.024</v>
       </c>
       <c r="I10" t="n">
-        <v>0.575</v>
+        <v>0.279</v>
       </c>
       <c r="J10" t="n">
-        <v>192</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
-        <v>871</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -785,34 +785,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.002</v>
+        <v>1.005</v>
       </c>
       <c r="C11" t="n">
-        <v>0.98</v>
+        <v>0.975</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.975</v>
+        <v>-2.978</v>
       </c>
       <c r="E11" t="n">
-        <v>0.992</v>
+        <v>0.995</v>
       </c>
       <c r="F11" t="n">
-        <v>0.081</v>
+        <v>0.082</v>
       </c>
       <c r="G11" t="n">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="H11" t="n">
         <v>0.025</v>
       </c>
       <c r="I11" t="n">
-        <v>0.569</v>
+        <v>0.28</v>
       </c>
       <c r="J11" t="n">
-        <v>162</v>
+        <v>4</v>
       </c>
       <c r="K11" t="n">
-        <v>730</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -820,34 +820,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.001</v>
+        <v>1.005</v>
       </c>
       <c r="C12" t="n">
-        <v>0.984</v>
+        <v>0.977</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.971</v>
+        <v>-2.977</v>
       </c>
       <c r="E12" t="n">
-        <v>0.987</v>
+        <v>0.993</v>
       </c>
       <c r="F12" t="n">
         <v>0.077</v>
       </c>
       <c r="G12" t="n">
-        <v>0.036</v>
+        <v>0.034</v>
       </c>
       <c r="H12" t="n">
-        <v>0.029</v>
+        <v>0.023</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.28</v>
       </c>
       <c r="J12" t="n">
-        <v>142</v>
+        <v>5</v>
       </c>
       <c r="K12" t="n">
-        <v>633</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 04-21-2024 at 18:49
</commit_message>
<xml_diff>
--- a/experiment_3/output/output_latex.xlsx
+++ b/experiment_3/output/output_latex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,9 @@
       <c r="K1" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -494,9 +497,12 @@
         <v>0.295</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>0.219</v>
       </c>
       <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -529,9 +535,12 @@
         <v>0.356</v>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>0.181</v>
       </c>
       <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -564,9 +573,12 @@
         <v>0.437</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>0.148</v>
       </c>
       <c r="K4" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -599,9 +611,12 @@
         <v>0.511</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>0.133</v>
       </c>
       <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -634,9 +649,12 @@
         <v>0.48</v>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>0.108</v>
       </c>
       <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
         <v>2</v>
       </c>
     </row>
@@ -669,9 +687,12 @@
         <v>0.332</v>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>0.078</v>
       </c>
       <c r="K7" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" t="n">
         <v>2</v>
       </c>
     </row>
@@ -704,9 +725,12 @@
         <v>0.283</v>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
+        <v>0.059</v>
       </c>
       <c r="K8" t="n">
+        <v>3</v>
+      </c>
+      <c r="L8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -739,9 +763,12 @@
         <v>0.28</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>0.043</v>
       </c>
       <c r="K9" t="n">
+        <v>3</v>
+      </c>
+      <c r="L9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -774,9 +801,12 @@
         <v>0.279</v>
       </c>
       <c r="J10" t="n">
-        <v>3</v>
+        <v>0.042</v>
       </c>
       <c r="K10" t="n">
+        <v>3</v>
+      </c>
+      <c r="L10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -809,9 +839,12 @@
         <v>0.28</v>
       </c>
       <c r="J11" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="K11" t="n">
         <v>4</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>3</v>
       </c>
     </row>
@@ -844,9 +877,12 @@
         <v>0.28</v>
       </c>
       <c r="J12" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="K12" t="n">
         <v>5</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated on 05-22-2024 at 21:13
</commit_message>
<xml_diff>
--- a/experiment_3/output/output_latex.xlsx
+++ b/experiment_3/output/output_latex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,15 +458,6 @@
       <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -488,22 +479,13 @@
         <v>7.254</v>
       </c>
       <c r="G2" t="n">
-        <v>0.141</v>
+        <v>0.127</v>
       </c>
       <c r="H2" t="n">
-        <v>0.127</v>
+        <v>0.219</v>
       </c>
       <c r="I2" t="n">
         <v>0.295</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.219</v>
-      </c>
-      <c r="K2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -526,22 +508,13 @@
         <v>5.634</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.079</v>
       </c>
       <c r="H3" t="n">
-        <v>0.079</v>
+        <v>0.181</v>
       </c>
       <c r="I3" t="n">
         <v>0.356</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.181</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -564,22 +537,13 @@
         <v>4.181</v>
       </c>
       <c r="G4" t="n">
-        <v>0.115</v>
+        <v>0.105</v>
       </c>
       <c r="H4" t="n">
-        <v>0.105</v>
+        <v>0.148</v>
       </c>
       <c r="I4" t="n">
         <v>0.437</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="K4" t="n">
-        <v>3</v>
-      </c>
-      <c r="L4" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -602,22 +566,13 @@
         <v>3.145</v>
       </c>
       <c r="G5" t="n">
-        <v>0.161</v>
+        <v>0.152</v>
       </c>
       <c r="H5" t="n">
-        <v>0.152</v>
+        <v>0.133</v>
       </c>
       <c r="I5" t="n">
         <v>0.511</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="K5" t="n">
-        <v>3</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -640,22 +595,13 @@
         <v>2.218</v>
       </c>
       <c r="G6" t="n">
-        <v>0.156</v>
+        <v>0.127</v>
       </c>
       <c r="H6" t="n">
-        <v>0.127</v>
+        <v>0.108</v>
       </c>
       <c r="I6" t="n">
         <v>0.48</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.108</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -678,22 +624,13 @@
         <v>1.335</v>
       </c>
       <c r="G7" t="n">
-        <v>0.095</v>
+        <v>0.082</v>
       </c>
       <c r="H7" t="n">
-        <v>0.082</v>
+        <v>0.078</v>
       </c>
       <c r="I7" t="n">
         <v>0.332</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.078</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -716,22 +653,13 @@
         <v>0.576</v>
       </c>
       <c r="G8" t="n">
-        <v>0.065</v>
+        <v>0.054</v>
       </c>
       <c r="H8" t="n">
-        <v>0.054</v>
+        <v>0.059</v>
       </c>
       <c r="I8" t="n">
         <v>0.283</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="K8" t="n">
-        <v>3</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -754,22 +682,13 @@
         <v>0.091</v>
       </c>
       <c r="G9" t="n">
-        <v>0.031</v>
+        <v>0.023</v>
       </c>
       <c r="H9" t="n">
-        <v>0.023</v>
+        <v>0.043</v>
       </c>
       <c r="I9" t="n">
         <v>0.28</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="K9" t="n">
-        <v>3</v>
-      </c>
-      <c r="L9" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -792,22 +711,13 @@
         <v>0.08599999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.033</v>
+        <v>0.024</v>
       </c>
       <c r="H10" t="n">
-        <v>0.024</v>
+        <v>0.042</v>
       </c>
       <c r="I10" t="n">
         <v>0.279</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="K10" t="n">
-        <v>3</v>
-      </c>
-      <c r="L10" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -815,37 +725,28 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.005</v>
+        <v>1.002</v>
       </c>
       <c r="C11" t="n">
-        <v>0.975</v>
+        <v>0.98</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.978</v>
+        <v>-2.975</v>
       </c>
       <c r="E11" t="n">
-        <v>0.995</v>
+        <v>0.992</v>
       </c>
       <c r="F11" t="n">
-        <v>0.082</v>
+        <v>0.081</v>
       </c>
       <c r="G11" t="n">
-        <v>0.034</v>
+        <v>0.025</v>
       </c>
       <c r="H11" t="n">
-        <v>0.025</v>
+        <v>0.042</v>
       </c>
       <c r="I11" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="K11" t="n">
-        <v>4</v>
-      </c>
-      <c r="L11" t="n">
-        <v>3</v>
+        <v>0.282</v>
       </c>
     </row>
     <row r="12">
@@ -868,22 +769,13 @@
         <v>0.077</v>
       </c>
       <c r="G12" t="n">
-        <v>0.034</v>
+        <v>0.023</v>
       </c>
       <c r="H12" t="n">
-        <v>0.023</v>
+        <v>0.041</v>
       </c>
       <c r="I12" t="n">
         <v>0.28</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="K12" t="n">
-        <v>5</v>
-      </c>
-      <c r="L12" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>